<commit_message>
S-01082 - Complete review of MusicXML v3 documentation to identify elements that still need implementing.
Updated spreadsheet to reflect recent implementation work.
</commit_message>
<xml_diff>
--- a/imusant old/Documentation/MusicXMLv3_Elements_Reqs.xlsx
+++ b/imusant old/Documentation/MusicXMLv3_Elements_Reqs.xlsx
@@ -1410,7 +1410,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1418,216 +1418,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2049,11 +1839,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A2:G216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G144" sqref="G144"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2089,7 +1880,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" hidden="1">
       <c r="A3" t="s">
         <v>350</v>
       </c>
@@ -2109,7 +1900,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" hidden="1">
       <c r="A4" t="s">
         <v>350</v>
       </c>
@@ -2129,7 +1920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" hidden="1">
       <c r="A5" t="s">
         <v>350</v>
       </c>
@@ -2149,7 +1940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" hidden="1">
       <c r="A6" t="s">
         <v>350</v>
       </c>
@@ -2192,7 +1983,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" hidden="1">
       <c r="A8" t="s">
         <v>350</v>
       </c>
@@ -2212,7 +2003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" hidden="1">
       <c r="A9" t="s">
         <v>350</v>
       </c>
@@ -2232,7 +2023,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45">
+    <row r="10" spans="1:7" ht="45" hidden="1">
       <c r="A10" t="s">
         <v>350</v>
       </c>
@@ -2252,7 +2043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" hidden="1">
       <c r="A11" t="s">
         <v>350</v>
       </c>
@@ -2275,7 +2066,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" hidden="1">
       <c r="A12" t="s">
         <v>350</v>
       </c>
@@ -2295,7 +2086,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" hidden="1">
       <c r="A13" t="s">
         <v>350</v>
       </c>
@@ -2315,7 +2106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" hidden="1">
       <c r="A14" t="s">
         <v>350</v>
       </c>
@@ -2338,7 +2129,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30">
+    <row r="15" spans="1:7" ht="30" hidden="1">
       <c r="A15" t="s">
         <v>350</v>
       </c>
@@ -2358,7 +2149,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" hidden="1">
       <c r="A16" t="s">
         <v>350</v>
       </c>
@@ -2378,7 +2169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30">
+    <row r="17" spans="1:7" ht="30" hidden="1">
       <c r="A17" t="s">
         <v>350</v>
       </c>
@@ -2401,7 +2192,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30">
+    <row r="18" spans="1:7" ht="30" hidden="1">
       <c r="A18" t="s">
         <v>350</v>
       </c>
@@ -2421,7 +2212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30">
+    <row r="19" spans="1:7" ht="30" hidden="1">
       <c r="A19" t="s">
         <v>350</v>
       </c>
@@ -2441,7 +2232,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30">
+    <row r="20" spans="1:7" ht="30" hidden="1">
       <c r="A20" t="s">
         <v>350</v>
       </c>
@@ -2484,7 +2275,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" hidden="1">
       <c r="A22" t="s">
         <v>350</v>
       </c>
@@ -2507,7 +2298,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" hidden="1">
       <c r="A23" t="s">
         <v>350</v>
       </c>
@@ -2570,7 +2361,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30">
+    <row r="26" spans="1:7" ht="30" hidden="1">
       <c r="A26" t="s">
         <v>350</v>
       </c>
@@ -2593,7 +2384,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" hidden="1">
       <c r="A27" t="s">
         <v>350</v>
       </c>
@@ -2616,7 +2407,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" t="s">
         <v>350</v>
       </c>
@@ -2662,7 +2453,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" hidden="1">
       <c r="A30" t="s">
         <v>350</v>
       </c>
@@ -2685,7 +2476,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30">
+    <row r="31" spans="1:7" ht="30" hidden="1">
       <c r="A31" t="s">
         <v>350</v>
       </c>
@@ -2708,7 +2499,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" hidden="1">
       <c r="A32" t="s">
         <v>350</v>
       </c>
@@ -2731,7 +2522,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" hidden="1">
       <c r="A33" t="s">
         <v>350</v>
       </c>
@@ -2754,7 +2545,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" hidden="1">
       <c r="A34" t="s">
         <v>350</v>
       </c>
@@ -2777,7 +2568,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" hidden="1">
       <c r="A35" t="s">
         <v>350</v>
       </c>
@@ -2797,7 +2588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" hidden="1">
       <c r="A36" t="s">
         <v>350</v>
       </c>
@@ -2817,7 +2608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" hidden="1">
       <c r="A37" t="s">
         <v>350</v>
       </c>
@@ -2837,7 +2628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30">
+    <row r="38" spans="1:7" ht="30" hidden="1">
       <c r="A38" t="s">
         <v>350</v>
       </c>
@@ -2857,7 +2648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="30">
+    <row r="39" spans="1:7" ht="30" hidden="1">
       <c r="A39" t="s">
         <v>350</v>
       </c>
@@ -2877,7 +2668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="30">
+    <row r="40" spans="1:7" ht="30" hidden="1">
       <c r="A40" t="s">
         <v>350</v>
       </c>
@@ -2920,7 +2711,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30">
+    <row r="42" spans="1:7" ht="30" hidden="1">
       <c r="A42" t="s">
         <v>351</v>
       </c>
@@ -2943,7 +2734,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" hidden="1">
       <c r="A43" t="s">
         <v>352</v>
       </c>
@@ -2963,7 +2754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" hidden="1">
       <c r="A44" t="s">
         <v>352</v>
       </c>
@@ -3003,7 +2794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" hidden="1">
       <c r="A46" t="s">
         <v>351</v>
       </c>
@@ -3023,7 +2814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" hidden="1">
       <c r="A47" t="s">
         <v>351</v>
       </c>
@@ -3066,7 +2857,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="60">
+    <row r="49" spans="1:7" ht="60" hidden="1">
       <c r="A49" t="s">
         <v>352</v>
       </c>
@@ -3086,7 +2877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" hidden="1">
       <c r="A50" t="s">
         <v>352</v>
       </c>
@@ -3109,7 +2900,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" hidden="1">
       <c r="A51" t="s">
         <v>352</v>
       </c>
@@ -3132,7 +2923,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" hidden="1">
       <c r="A52" t="s">
         <v>352</v>
       </c>
@@ -3155,7 +2946,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" hidden="1">
       <c r="A53" t="s">
         <v>352</v>
       </c>
@@ -3175,7 +2966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" hidden="1">
       <c r="A54" t="s">
         <v>352</v>
       </c>
@@ -3195,7 +2986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" hidden="1">
       <c r="A55" t="s">
         <v>352</v>
       </c>
@@ -3307,7 +3098,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" hidden="1">
       <c r="A60" t="s">
         <v>352</v>
       </c>
@@ -3327,7 +3118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" hidden="1">
       <c r="A61" t="s">
         <v>352</v>
       </c>
@@ -3347,7 +3138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" hidden="1">
       <c r="A62" t="s">
         <v>352</v>
       </c>
@@ -3367,7 +3158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" hidden="1">
       <c r="A63" t="s">
         <v>352</v>
       </c>
@@ -3387,7 +3178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" hidden="1">
       <c r="A64" t="s">
         <v>352</v>
       </c>
@@ -3407,7 +3198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" hidden="1">
       <c r="A65" t="s">
         <v>352</v>
       </c>
@@ -3427,7 +3218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" hidden="1">
       <c r="A66" t="s">
         <v>352</v>
       </c>
@@ -3447,7 +3238,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="45">
+    <row r="67" spans="1:7" ht="45" hidden="1">
       <c r="A67" t="s">
         <v>352</v>
       </c>
@@ -3470,7 +3261,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" hidden="1">
       <c r="A68" t="s">
         <v>352</v>
       </c>
@@ -3490,7 +3281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" hidden="1">
       <c r="A69" t="s">
         <v>352</v>
       </c>
@@ -3510,7 +3301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" hidden="1">
       <c r="A70" t="s">
         <v>352</v>
       </c>
@@ -3530,7 +3321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" hidden="1">
       <c r="A71" t="s">
         <v>352</v>
       </c>
@@ -3550,7 +3341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" hidden="1">
       <c r="A72" t="s">
         <v>352</v>
       </c>
@@ -3570,7 +3361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" hidden="1">
       <c r="A73" t="s">
         <v>352</v>
       </c>
@@ -3590,7 +3381,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="60">
+    <row r="74" spans="1:7" ht="60" hidden="1">
       <c r="A74" t="s">
         <v>353</v>
       </c>
@@ -3613,7 +3404,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="30">
+    <row r="75" spans="1:7" ht="30" hidden="1">
       <c r="A75" t="s">
         <v>354</v>
       </c>
@@ -3636,7 +3427,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="30">
+    <row r="76" spans="1:7" ht="30" hidden="1">
       <c r="A76" t="s">
         <v>353</v>
       </c>
@@ -3659,7 +3450,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="45">
+    <row r="77" spans="1:7" ht="45" hidden="1">
       <c r="A77" t="s">
         <v>353</v>
       </c>
@@ -3679,7 +3470,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="30">
+    <row r="78" spans="1:7" ht="30" hidden="1">
       <c r="A78" t="s">
         <v>355</v>
       </c>
@@ -3699,7 +3490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" hidden="1">
       <c r="A79" t="s">
         <v>355</v>
       </c>
@@ -3722,7 +3513,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="30">
+    <row r="80" spans="1:7" ht="30" hidden="1">
       <c r="A80" t="s">
         <v>355</v>
       </c>
@@ -3742,7 +3533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" hidden="1">
       <c r="A81" t="s">
         <v>355</v>
       </c>
@@ -3762,7 +3553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" hidden="1">
       <c r="A82" t="s">
         <v>355</v>
       </c>
@@ -3782,7 +3573,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" hidden="1">
       <c r="A83" t="s">
         <v>355</v>
       </c>
@@ -3802,7 +3593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" hidden="1">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -3825,7 +3616,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" hidden="1">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -3845,7 +3636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" hidden="1">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -3868,7 +3659,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="30">
+    <row r="87" spans="1:7" ht="30" hidden="1">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -3888,7 +3679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" hidden="1">
       <c r="A88" t="s">
         <v>8</v>
       </c>
@@ -3911,7 +3702,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" hidden="1">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -3931,7 +3722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" hidden="1">
       <c r="A90" t="s">
         <v>8</v>
       </c>
@@ -3951,7 +3742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" hidden="1">
       <c r="A91" t="s">
         <v>8</v>
       </c>
@@ -3974,7 +3765,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="30">
+    <row r="92" spans="1:7" ht="30" hidden="1">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -3994,7 +3785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="30">
+    <row r="93" spans="1:7" ht="30" hidden="1">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -4014,7 +3805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" hidden="1">
       <c r="A94" t="s">
         <v>8</v>
       </c>
@@ -4034,7 +3825,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" hidden="1">
       <c r="A95" t="s">
         <v>8</v>
       </c>
@@ -4054,7 +3845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="60">
+    <row r="96" spans="1:7" ht="60" hidden="1">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -4077,7 +3868,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" hidden="1">
       <c r="A97" t="s">
         <v>8</v>
       </c>
@@ -4097,7 +3888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" hidden="1">
       <c r="A98" t="s">
         <v>8</v>
       </c>
@@ -4117,7 +3908,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" hidden="1">
       <c r="A99" t="s">
         <v>8</v>
       </c>
@@ -4137,7 +3928,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" hidden="1">
       <c r="A100" t="s">
         <v>8</v>
       </c>
@@ -4177,7 +3968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" hidden="1">
       <c r="A102" t="s">
         <v>8</v>
       </c>
@@ -4197,7 +3988,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="30">
+    <row r="103" spans="1:6" ht="30" hidden="1">
       <c r="A103" t="s">
         <v>8</v>
       </c>
@@ -4217,7 +4008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="30">
+    <row r="104" spans="1:6" ht="30" hidden="1">
       <c r="A104" t="s">
         <v>8</v>
       </c>
@@ -4237,7 +4028,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" hidden="1">
       <c r="A105" t="s">
         <v>8</v>
       </c>
@@ -4257,7 +4048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="30">
+    <row r="106" spans="1:6" ht="30" hidden="1">
       <c r="A106" t="s">
         <v>8</v>
       </c>
@@ -4277,7 +4068,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" hidden="1">
       <c r="A107" t="s">
         <v>8</v>
       </c>
@@ -4297,7 +4088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" hidden="1">
       <c r="A108" t="s">
         <v>8</v>
       </c>
@@ -4317,7 +4108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="45">
+    <row r="109" spans="1:6" ht="45" hidden="1">
       <c r="A109" t="s">
         <v>8</v>
       </c>
@@ -4337,7 +4128,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" hidden="1">
       <c r="A110" t="s">
         <v>8</v>
       </c>
@@ -4357,7 +4148,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" hidden="1">
       <c r="A111" t="s">
         <v>8</v>
       </c>
@@ -4377,7 +4168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" hidden="1">
       <c r="A112" t="s">
         <v>8</v>
       </c>
@@ -4397,7 +4188,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" hidden="1">
       <c r="A113" t="s">
         <v>8</v>
       </c>
@@ -4420,7 +4211,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" hidden="1">
       <c r="A114" t="s">
         <v>8</v>
       </c>
@@ -4440,7 +4231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" hidden="1">
       <c r="A115" t="s">
         <v>8</v>
       </c>
@@ -4460,7 +4251,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" hidden="1">
       <c r="A116" t="s">
         <v>8</v>
       </c>
@@ -4483,7 +4274,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" hidden="1">
       <c r="A117" t="s">
         <v>8</v>
       </c>
@@ -4506,7 +4297,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" hidden="1">
       <c r="A118" t="s">
         <v>8</v>
       </c>
@@ -4527,7 +4318,7 @@
       </c>
       <c r="G118" s="7"/>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" hidden="1">
       <c r="A119" t="s">
         <v>8</v>
       </c>
@@ -4548,7 +4339,7 @@
       </c>
       <c r="G119" s="7"/>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" hidden="1">
       <c r="A120" t="s">
         <v>8</v>
       </c>
@@ -4584,13 +4375,13 @@
         <v>9</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G121" s="7" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" hidden="1">
       <c r="A122" t="s">
         <v>8</v>
       </c>
@@ -4611,7 +4402,7 @@
       </c>
       <c r="G122" s="7"/>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" hidden="1">
       <c r="A123" t="s">
         <v>8</v>
       </c>
@@ -4632,7 +4423,7 @@
       </c>
       <c r="G123" s="7"/>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" hidden="1">
       <c r="A124" t="s">
         <v>8</v>
       </c>
@@ -4653,7 +4444,7 @@
       </c>
       <c r="G124" s="7"/>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" hidden="1">
       <c r="A125" t="s">
         <v>8</v>
       </c>
@@ -4674,7 +4465,7 @@
       </c>
       <c r="G125" s="7"/>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" hidden="1">
       <c r="A126" t="s">
         <v>8</v>
       </c>
@@ -4695,7 +4486,7 @@
       </c>
       <c r="G126" s="7"/>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" hidden="1">
       <c r="A127" t="s">
         <v>8</v>
       </c>
@@ -4716,7 +4507,7 @@
       </c>
       <c r="G127" s="7"/>
     </row>
-    <row r="128" spans="1:7" ht="30">
+    <row r="128" spans="1:7" ht="30" hidden="1">
       <c r="A128" t="s">
         <v>8</v>
       </c>
@@ -4737,7 +4528,7 @@
       </c>
       <c r="G128" s="7"/>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" hidden="1">
       <c r="A129" t="s">
         <v>8</v>
       </c>
@@ -4758,7 +4549,7 @@
       </c>
       <c r="G129" s="7"/>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" hidden="1">
       <c r="A130" t="s">
         <v>8</v>
       </c>
@@ -4779,7 +4570,7 @@
       </c>
       <c r="G130" s="7"/>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" hidden="1">
       <c r="A131" t="s">
         <v>8</v>
       </c>
@@ -4800,7 +4591,7 @@
       </c>
       <c r="G131" s="7"/>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" hidden="1">
       <c r="A132" t="s">
         <v>8</v>
       </c>
@@ -4821,7 +4612,7 @@
       </c>
       <c r="G132" s="7"/>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" hidden="1">
       <c r="A133" t="s">
         <v>8</v>
       </c>
@@ -4863,7 +4654,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" hidden="1">
       <c r="A135" t="s">
         <v>8</v>
       </c>
@@ -4884,7 +4675,7 @@
       </c>
       <c r="G135" s="7"/>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" hidden="1">
       <c r="A136" t="s">
         <v>8</v>
       </c>
@@ -4928,7 +4719,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" hidden="1">
       <c r="A138" t="s">
         <v>8</v>
       </c>
@@ -4949,7 +4740,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="30">
+    <row r="139" spans="1:7" ht="30" hidden="1">
       <c r="A139" t="s">
         <v>8</v>
       </c>
@@ -4970,7 +4761,7 @@
       </c>
       <c r="G139" s="7"/>
     </row>
-    <row r="140" spans="1:7" ht="60">
+    <row r="140" spans="1:7" ht="60" hidden="1">
       <c r="A140" t="s">
         <v>8</v>
       </c>
@@ -4991,7 +4782,7 @@
       </c>
       <c r="G140" s="7"/>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" hidden="1">
       <c r="A141" t="s">
         <v>8</v>
       </c>
@@ -5010,7 +4801,7 @@
       </c>
       <c r="G141" s="7"/>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" hidden="1">
       <c r="A142" t="s">
         <v>8</v>
       </c>
@@ -5031,7 +4822,7 @@
       </c>
       <c r="G142" s="7"/>
     </row>
-    <row r="143" spans="1:7" ht="285">
+    <row r="143" spans="1:7" ht="285" hidden="1">
       <c r="A143" t="s">
         <v>8</v>
       </c>
@@ -5054,7 +4845,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" hidden="1">
       <c r="A144" t="s">
         <v>8</v>
       </c>
@@ -5074,7 +4865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="30">
+    <row r="145" spans="1:7" ht="30" hidden="1">
       <c r="A145" t="s">
         <v>8</v>
       </c>
@@ -5094,7 +4885,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" hidden="1">
       <c r="A146" t="s">
         <v>8</v>
       </c>
@@ -5114,7 +4905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" hidden="1">
       <c r="A147" t="s">
         <v>8</v>
       </c>
@@ -5134,7 +4925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" hidden="1">
       <c r="A148" t="s">
         <v>8</v>
       </c>
@@ -5154,7 +4945,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" hidden="1">
       <c r="A149" t="s">
         <v>8</v>
       </c>
@@ -5177,7 +4968,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" hidden="1">
       <c r="A150" t="s">
         <v>8</v>
       </c>
@@ -5214,13 +5005,13 @@
         <v>9</v>
       </c>
       <c r="F151" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G151" s="7" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" hidden="1">
       <c r="A152" t="s">
         <v>8</v>
       </c>
@@ -5240,7 +5031,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" hidden="1">
       <c r="A153" t="s">
         <v>8</v>
       </c>
@@ -5260,7 +5051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" hidden="1">
       <c r="A154" t="s">
         <v>8</v>
       </c>
@@ -5280,7 +5071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" hidden="1">
       <c r="A155" t="s">
         <v>8</v>
       </c>
@@ -5300,7 +5091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" hidden="1">
       <c r="A156" t="s">
         <v>8</v>
       </c>
@@ -5320,7 +5111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" hidden="1">
       <c r="A157" t="s">
         <v>8</v>
       </c>
@@ -5340,7 +5131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" hidden="1">
       <c r="A158" t="s">
         <v>8</v>
       </c>
@@ -5360,7 +5151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" hidden="1">
       <c r="A159" t="s">
         <v>8</v>
       </c>
@@ -5380,7 +5171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" hidden="1">
       <c r="A160" t="s">
         <v>8</v>
       </c>
@@ -5400,7 +5191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" hidden="1">
       <c r="A161" t="s">
         <v>8</v>
       </c>
@@ -5420,7 +5211,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" hidden="1">
       <c r="A162" t="s">
         <v>8</v>
       </c>
@@ -5440,7 +5231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" hidden="1">
       <c r="A163" t="s">
         <v>8</v>
       </c>
@@ -5460,7 +5251,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" hidden="1">
       <c r="A164" t="s">
         <v>8</v>
       </c>
@@ -5480,7 +5271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" hidden="1">
       <c r="A165" t="s">
         <v>8</v>
       </c>
@@ -5523,7 +5314,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" hidden="1">
       <c r="A167" t="s">
         <v>8</v>
       </c>
@@ -5543,7 +5334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="165">
+    <row r="168" spans="1:7" ht="165" hidden="1">
       <c r="A168" t="s">
         <v>8</v>
       </c>
@@ -5566,7 +5357,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" hidden="1">
       <c r="A169" t="s">
         <v>8</v>
       </c>
@@ -5609,7 +5400,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" hidden="1">
       <c r="A171" t="s">
         <v>8</v>
       </c>
@@ -5629,7 +5420,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" hidden="1">
       <c r="A172" t="s">
         <v>8</v>
       </c>
@@ -5652,7 +5443,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" hidden="1">
       <c r="A173" t="s">
         <v>8</v>
       </c>
@@ -5672,7 +5463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" hidden="1">
       <c r="A174" t="s">
         <v>8</v>
       </c>
@@ -5692,7 +5483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" hidden="1">
       <c r="A175" t="s">
         <v>8</v>
       </c>
@@ -5712,7 +5503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" hidden="1">
       <c r="A176" t="s">
         <v>8</v>
       </c>
@@ -5732,7 +5523,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="30">
+    <row r="177" spans="1:7" ht="30" hidden="1">
       <c r="A177" t="s">
         <v>8</v>
       </c>
@@ -5752,7 +5543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" hidden="1">
       <c r="A178" t="s">
         <v>8</v>
       </c>
@@ -5772,7 +5563,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" hidden="1">
       <c r="A179" t="s">
         <v>8</v>
       </c>
@@ -5815,7 +5606,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" hidden="1">
       <c r="A181" t="s">
         <v>8</v>
       </c>
@@ -5835,7 +5626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" hidden="1">
       <c r="A182" t="s">
         <v>8</v>
       </c>
@@ -5872,13 +5663,13 @@
         <v>9</v>
       </c>
       <c r="F183" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G183" s="7" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" hidden="1">
       <c r="A184" t="s">
         <v>8</v>
       </c>
@@ -5898,7 +5689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="30">
+    <row r="185" spans="1:7" ht="30" hidden="1">
       <c r="A185" t="s">
         <v>8</v>
       </c>
@@ -5918,7 +5709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" hidden="1">
       <c r="A186" t="s">
         <v>356</v>
       </c>
@@ -5938,7 +5729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" hidden="1">
       <c r="A187" t="s">
         <v>356</v>
       </c>
@@ -5958,7 +5749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" hidden="1">
       <c r="A188" t="s">
         <v>356</v>
       </c>
@@ -5978,7 +5769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" hidden="1">
       <c r="A189" t="s">
         <v>356</v>
       </c>
@@ -5998,7 +5789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="30">
+    <row r="190" spans="1:7" ht="30" hidden="1">
       <c r="A190" t="s">
         <v>356</v>
       </c>
@@ -6018,7 +5809,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" hidden="1">
       <c r="A191" t="s">
         <v>356</v>
       </c>
@@ -6038,7 +5829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" hidden="1">
       <c r="A192" t="s">
         <v>356</v>
       </c>
@@ -6058,7 +5849,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" hidden="1">
       <c r="A193" t="s">
         <v>356</v>
       </c>
@@ -6078,7 +5869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" hidden="1">
       <c r="A194" t="s">
         <v>356</v>
       </c>
@@ -6118,7 +5909,7 @@
         <v>9</v>
       </c>
       <c r="F195" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="196" spans="1:7">
@@ -6138,13 +5929,13 @@
         <v>9</v>
       </c>
       <c r="F196" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G196" s="7" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" hidden="1">
       <c r="A197" t="s">
         <v>356</v>
       </c>
@@ -6164,7 +5955,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="30">
+    <row r="198" spans="1:7" ht="30" hidden="1">
       <c r="A198" t="s">
         <v>356</v>
       </c>
@@ -6184,7 +5975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" hidden="1">
       <c r="A199" t="s">
         <v>356</v>
       </c>
@@ -6204,7 +5995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:7" hidden="1">
       <c r="A200" t="s">
         <v>356</v>
       </c>
@@ -6224,7 +6015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="201" spans="1:7">
+    <row r="201" spans="1:7" hidden="1">
       <c r="A201" t="s">
         <v>356</v>
       </c>
@@ -6244,7 +6035,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="202" spans="1:7">
+    <row r="202" spans="1:7" hidden="1">
       <c r="A202" t="s">
         <v>356</v>
       </c>
@@ -6264,7 +6055,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:7" hidden="1">
       <c r="A203" t="s">
         <v>356</v>
       </c>
@@ -6281,7 +6072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:7">
+    <row r="204" spans="1:7" hidden="1">
       <c r="A204" t="s">
         <v>356</v>
       </c>
@@ -6318,7 +6109,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206" spans="1:7">
+    <row r="206" spans="1:7" hidden="1">
       <c r="A206" t="s">
         <v>356</v>
       </c>
@@ -6335,7 +6126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="207" spans="1:7">
+    <row r="207" spans="1:7" hidden="1">
       <c r="A207" t="s">
         <v>356</v>
       </c>
@@ -6355,7 +6146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:7">
+    <row r="208" spans="1:7" hidden="1">
       <c r="A208" t="s">
         <v>356</v>
       </c>
@@ -6375,7 +6166,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="209" spans="1:6">
+    <row r="209" spans="1:6" hidden="1">
       <c r="A209" t="s">
         <v>356</v>
       </c>
@@ -6395,7 +6186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="1:6">
+    <row r="210" spans="1:6" hidden="1">
       <c r="A210" t="s">
         <v>356</v>
       </c>
@@ -6415,7 +6206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211" spans="1:6">
+    <row r="211" spans="1:6" hidden="1">
       <c r="A211" t="s">
         <v>356</v>
       </c>
@@ -6435,7 +6226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="1:6">
+    <row r="212" spans="1:6" hidden="1">
       <c r="A212" t="s">
         <v>356</v>
       </c>
@@ -6455,7 +6246,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:6">
+    <row r="213" spans="1:6" hidden="1">
       <c r="A213" t="s">
         <v>356</v>
       </c>
@@ -6492,7 +6283,7 @@
         <v>9</v>
       </c>
       <c r="F214" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="215" spans="1:6">
@@ -6512,10 +6303,10 @@
         <v>9</v>
       </c>
       <c r="F215" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" hidden="1">
       <c r="A216" t="s">
         <v>356</v>
       </c>
@@ -6536,15 +6327,26 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G216"/>
+  <autoFilter ref="A2:G216">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="y"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="n"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="D3:F216 G7 G17 G20 G22">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>AND(D3="y", F3="n")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>AND(D3="m", F3="n")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(D3="y", F3="y")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Reviewed MusicXMLv3_Elements_reqs as per S-01082
</commit_message>
<xml_diff>
--- a/imusant old/Documentation/MusicXMLv3_Elements_Reqs.xlsx
+++ b/imusant old/Documentation/MusicXMLv3_Elements_Reqs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="20" windowWidth="36420" windowHeight="21080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1100" yWindow="20" windowWidth="36420" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="422">
   <si>
     <t>Element</t>
   </si>
@@ -1324,6 +1324,12 @@
   </si>
   <si>
     <t xml:space="preserve">Works are optionally identified by number and title. </t>
+  </si>
+  <si>
+    <t>Reviewed: 1 February 2016</t>
+  </si>
+  <si>
+    <t>Reviewed by: Jason Stoessel</t>
   </si>
 </sst>
 </file>
@@ -1768,10 +1774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:A16"/>
+  <dimension ref="A4:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1822,6 +1828,16 @@
     <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>406</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -1842,9 +1858,9 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A2:G216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F151" sqref="F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1977,7 +1993,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>411</v>
@@ -2272,7 +2288,7 @@
         <v>9</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:7" hidden="1">
@@ -2447,7 +2463,7 @@
         <v>9</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>61</v>
@@ -2851,7 +2867,7 @@
         <v>9</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G48" s="7" t="s">
         <v>100</v>
@@ -3023,7 +3039,7 @@
         <v>9</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G56" s="7" t="s">
         <v>119</v>
@@ -3046,7 +3062,7 @@
         <v>12</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G57" s="7" t="s">
         <v>123</v>
@@ -3069,7 +3085,7 @@
         <v>9</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G58" s="7" t="s">
         <v>127</v>
@@ -3092,7 +3108,7 @@
         <v>9</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G59" s="7" t="s">
         <v>130</v>
@@ -3965,7 +3981,7 @@
         <v>9</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:6" hidden="1">
@@ -4648,7 +4664,7 @@
         <v>9</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G134" s="7" t="s">
         <v>275</v>
@@ -4713,7 +4729,7 @@
         <v>9</v>
       </c>
       <c r="F137" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G137" s="7" t="s">
         <v>281</v>
@@ -5308,7 +5324,7 @@
         <v>9</v>
       </c>
       <c r="F166" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G166" s="7" t="s">
         <v>314</v>
@@ -5394,7 +5410,7 @@
         <v>9</v>
       </c>
       <c r="F170" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G170" s="7" t="s">
         <v>323</v>

</xml_diff>